<commit_message>
The final countdown for the near infrared
</commit_message>
<xml_diff>
--- a/Project/IAG Solar Flux Atlas/Infrared range/Data/new_values_fe.xlsx
+++ b/Project/IAG Solar Flux Atlas/Infrared range/Data/new_values_fe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Infrared range\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clauw\Documents\Programming\Final-Project\Project\IAG Solar Flux Atlas\Infrared range\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F31AF2E-3AC1-4FCA-9950-873743AA851D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C098EFD-D450-4B9D-AC49-F0B5B6564756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,12 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B192"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,958 +396,783 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>10035.609399999999</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>10067.804700000001</v>
+      <c r="A3">
+        <v>10084.1584</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>10084.1584</v>
+      <c r="A4">
+        <v>10116.789199999999</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>10087.840899999999</v>
+      <c r="A5">
+        <v>10139.8807</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>10092.541499999999</v>
+      <c r="A6">
+        <v>10145.6242</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>10116.789199999999</v>
+      <c r="A7">
+        <v>10148.3444</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>10139.8807</v>
+      <c r="A8">
+        <v>10157.949000000001</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>10145.6242</v>
+      <c r="A9">
+        <v>10170.2562</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>10148.3444</v>
+      <c r="A10">
+        <v>10219.1142</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>10157.949000000001</v>
+      <c r="A11">
+        <v>10221.211499999999</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>10170.2562</v>
+      <c r="A12">
+        <v>10268.0337</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>10219.1142</v>
+      <c r="A13">
+        <v>10310.2796</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>10221.211499999999</v>
+      <c r="A14">
+        <v>10335.161</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>10268.0337</v>
+      <c r="A15">
+        <v>10343.720799999999</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>10286.5969</v>
+      <c r="A16">
+        <v>10348.019399999999</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>10310.2796</v>
+      <c r="A17">
+        <v>10350.802100000001</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>10335.161</v>
+      <c r="A18">
+        <v>10365.544</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>10343.720799999999</v>
+      <c r="A19">
+        <v>10381.8464</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>10348.019399999999</v>
+      <c r="A20">
+        <v>10391.5915</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>10350.802100000001</v>
+      <c r="A21">
+        <v>10398.646699999999</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>10356.6445</v>
+      <c r="A22">
+        <v>10425.8871</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>10365.544</v>
+      <c r="A23">
+        <v>10426.6023</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>10381.8464</v>
+      <c r="A24">
+        <v>10472.5234</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>10391.5915</v>
+      <c r="A25">
+        <v>10535.121999999999</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>10398.646699999999</v>
+      <c r="A26">
+        <v>10558.543799999999</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>10425.8871</v>
+      <c r="A27">
+        <v>10580.039000000001</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>10426.6023</v>
+      <c r="A28">
+        <v>10619.6322</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>10472.5234</v>
+      <c r="A29">
+        <v>10755.953100000001</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>10535.121999999999</v>
+      <c r="A30">
+        <v>10783.6477</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>10558.543799999999</v>
+      <c r="A31">
+        <v>10786.005300000001</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>10580.039000000001</v>
+      <c r="A32">
+        <v>10821.240100000001</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>10619.6322</v>
+      <c r="A33">
+        <v>10887.246300000001</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>10755.953100000001</v>
+      <c r="A34">
+        <v>10899.2871</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>10783.6477</v>
+      <c r="A35">
+        <v>11122.843199999999</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>10786.005300000001</v>
+      <c r="A36">
+        <v>11672.836499999999</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>10821.240100000001</v>
+      <c r="A37">
+        <v>11887.3385</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>10887.246300000001</v>
+      <c r="A38">
+        <v>11893.7446</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>10899.2871</v>
+      <c r="A39">
+        <v>12056.3824</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>11029.8104</v>
+      <c r="A40">
+        <v>12134.4953</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>11122.843199999999</v>
+      <c r="A41">
+        <v>12216.6754</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <v>11391.6585</v>
+      <c r="A42">
+        <v>12230.459000000001</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>11405.8406</v>
+      <c r="A43">
+        <v>12343.864</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>11672.836499999999</v>
+      <c r="A44">
+        <v>12346.291800000001</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>11887.3385</v>
+      <c r="A45">
+        <v>12560.434499999999</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>11893.7446</v>
+      <c r="A46">
+        <v>12619.377699999999</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>12056.3824</v>
+      <c r="A47">
+        <v>12642.1643</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>12134.4953</v>
+      <c r="A48">
+        <v>12810.6535</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>12216.6754</v>
+      <c r="A49">
+        <v>12828.3694</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>12230.459000000001</v>
+      <c r="A50">
+        <v>12844.0867</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>12343.864</v>
+      <c r="A51">
+        <v>12883.2924</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>12346.291800000001</v>
+      <c r="A52">
+        <v>12936.5437</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>12513.9421</v>
+      <c r="A53">
+        <v>13355.828100000001</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>12560.434499999999</v>
+      <c r="A54">
+        <v>13395.7647</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>12619.377699999999</v>
+      <c r="A55">
+        <v>14812.3724</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>12642.1643</v>
+      <c r="A56">
+        <v>14960.2394</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>12652.202799999999</v>
+      <c r="A57">
+        <v>15021.806399999999</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>12810.6535</v>
+      <c r="A58">
+        <v>15055.862499999999</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>12828.3694</v>
+      <c r="A59">
+        <v>15098.8248</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>12844.0867</v>
+      <c r="A60">
+        <v>15126.515100000001</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>12883.2924</v>
+      <c r="A61">
+        <v>15180.864799999999</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>12936.5437</v>
+      <c r="A62">
+        <v>15211.686600000001</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>13355.828100000001</v>
+      <c r="A63">
+        <v>15223.781999999999</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>13395.7647</v>
+      <c r="A64">
+        <v>15228.891799999999</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>14812.3724</v>
+      <c r="A65">
+        <v>15249.1397</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>14901.4818</v>
+      <c r="A66">
+        <v>15250.665300000001</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>14960.2394</v>
+      <c r="A67">
+        <v>15339.5784</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>14993.1556</v>
+      <c r="A68">
+        <v>15347.9951</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>15021.806399999999</v>
+      <c r="A69">
+        <v>15494.572</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>15055.862499999999</v>
+      <c r="A70">
+        <v>15518.5211</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>15098.8248</v>
+      <c r="A71">
+        <v>15523.606599999999</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>15126.515100000001</v>
+      <c r="A72">
+        <v>15536.003000000001</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>15180.864799999999</v>
+      <c r="A73">
+        <v>15538.491900000001</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>15211.686600000001</v>
+      <c r="A74">
+        <v>15546.3307</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>15223.781999999999</v>
+      <c r="A75">
+        <v>15555.684800000001</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>15228.891799999999</v>
+      <c r="A76">
+        <v>15592.5237</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>15249.1397</v>
+      <c r="A77">
+        <v>15603.138499999999</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>15250.665300000001</v>
+      <c r="A78">
+        <v>15615.4038</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>15255.1764</v>
+      <c r="A79">
+        <v>15617.8987</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>15300.345799999999</v>
+      <c r="A80">
+        <v>15625.927799999999</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>15339.5784</v>
+      <c r="A81">
+        <v>15636.2214</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>15347.9951</v>
+      <c r="A82">
+        <v>15652.790999999999</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
-        <v>15494.572</v>
+      <c r="A83">
+        <v>15657.151</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>15518.5211</v>
+      <c r="A84">
+        <v>15666.2978</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>15523.606599999999</v>
+      <c r="A85">
+        <v>15669.525900000001</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <v>15536.003000000001</v>
+      <c r="A86">
+        <v>15680.8729</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
-        <v>15538.491900000001</v>
+      <c r="A87">
+        <v>15681.8073</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="2">
-        <v>15546.3307</v>
+      <c r="A88">
+        <v>15686.803599999999</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="2">
-        <v>15555.684800000001</v>
+      <c r="A89">
+        <v>15690.731900000001</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
-        <v>15570.9833</v>
+      <c r="A90">
+        <v>15696.145200000001</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
-        <v>15592.5237</v>
+      <c r="A91">
+        <v>15727.8899</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2">
-        <v>15594.3109</v>
+      <c r="A92">
+        <v>15778.3807</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
-        <v>15603.138499999999</v>
+      <c r="A93">
+        <v>15793.3148</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
-        <v>15615.4038</v>
+      <c r="A94">
+        <v>15820.957399999999</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
-        <v>15617.8987</v>
+      <c r="A95">
+        <v>15822.464400000001</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2">
-        <v>15625.927799999999</v>
+      <c r="A96">
+        <v>15823.460800000001</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="2">
-        <v>15636.2214</v>
+      <c r="A97">
+        <v>15826.0352</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="2">
-        <v>15649.2955</v>
+      <c r="A98">
+        <v>15827.1448</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="2">
-        <v>15652.790999999999</v>
+      <c r="A99">
+        <v>15839.4915</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="2">
-        <v>15657.151</v>
+      <c r="A100">
+        <v>15857.651599999999</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
-        <v>15666.2978</v>
+      <c r="A101">
+        <v>15868.0489</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="2">
-        <v>15669.525900000001</v>
+      <c r="A102">
+        <v>15872.8622</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2">
-        <v>15680.8729</v>
+      <c r="A103">
+        <v>15882.7876</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>15681.8073</v>
+      <c r="A104">
+        <v>15899.573200000001</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2">
-        <v>15686.803599999999</v>
+      <c r="A105">
+        <v>15905.865299999999</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
-        <v>15690.731900000001</v>
+      <c r="A106">
+        <v>15910.390100000001</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>15696.145200000001</v>
+      <c r="A107">
+        <v>15915.652099999999</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>15727.8899</v>
+      <c r="A108">
+        <v>15975.617399999999</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="2">
-        <v>15778.3807</v>
+      <c r="A109">
+        <v>15985.0942</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="2">
-        <v>15793.3148</v>
+      <c r="A110">
+        <v>16002.0995</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
-        <v>15810.6016</v>
+      <c r="A111">
+        <v>16013.989799999999</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2">
-        <v>15820.957399999999</v>
+      <c r="A112">
+        <v>16033.801799999999</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="2">
-        <v>15822.464400000001</v>
+      <c r="A113">
+        <v>16045.0391</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="2">
-        <v>15823.460800000001</v>
+      <c r="A114">
+        <v>16075.7929</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="2">
-        <v>15826.0352</v>
+      <c r="A115">
+        <v>16080.3141</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="2">
-        <v>15827.1448</v>
+      <c r="A116">
+        <v>16093.131600000001</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="2">
-        <v>15839.4915</v>
+      <c r="A117">
+        <v>16160.9789</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2">
-        <v>15844.5234</v>
+      <c r="A118">
+        <v>16179.397199999999</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="2">
-        <v>15857.651599999999</v>
+      <c r="A119">
+        <v>16185.331099999999</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="2">
-        <v>15868.0489</v>
+      <c r="A120">
+        <v>16199.486999999999</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>15868.985699999999</v>
+      <c r="A121">
+        <v>16202.930700000001</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="2">
-        <v>15872.8622</v>
+      <c r="A122">
+        <v>16208.682199999999</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2">
-        <v>15882.7876</v>
+      <c r="A123">
+        <v>16212.1746</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="2">
-        <v>15895.5093</v>
+      <c r="A124">
+        <v>16230.056500000001</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>15899.573200000001</v>
+      <c r="A125">
+        <v>16236.088299999999</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="2">
-        <v>15905.865299999999</v>
+      <c r="A126">
+        <v>16240.4048</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="2">
-        <v>15910.390100000001</v>
+      <c r="A127">
+        <v>16250.900900000001</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
-        <v>15915.652099999999</v>
+      <c r="A128">
+        <v>16289.221</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2">
-        <v>15938.375899999999</v>
+      <c r="A129">
+        <v>16297.299199999999</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>15966.9216</v>
+      <c r="A130">
+        <v>16320.782999999999</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
-        <v>15975.617399999999</v>
+      <c r="A131">
+        <v>16323.1594</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="2">
-        <v>15985.0942</v>
+      <c r="A132">
+        <v>16335.9908</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="2">
-        <v>16002.0995</v>
+      <c r="A133">
+        <v>16388.6201</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2">
-        <v>16013.989799999999</v>
+      <c r="A134">
+        <v>16398.8704</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="2">
-        <v>16033.801799999999</v>
+      <c r="A135">
+        <v>16409.082399999999</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="2">
-        <v>16045.0391</v>
+      <c r="A136">
+        <v>16441.1165</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="2">
-        <v>16075.7929</v>
+      <c r="A137">
+        <v>16444.893599999999</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="2">
-        <v>16080.3141</v>
+      <c r="A138">
+        <v>16449.311000000002</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="2">
-        <v>16093.131600000001</v>
+      <c r="A139">
+        <v>16491.1731</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="2">
-        <v>16160.9789</v>
+      <c r="A140">
+        <v>16521.740699999998</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="2">
-        <v>16179.397199999999</v>
+      <c r="A141">
+        <v>16543.713800000001</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="2">
-        <v>16185.331099999999</v>
+      <c r="A142">
+        <v>16556.518899999999</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="2">
-        <v>16199.486999999999</v>
+      <c r="A143">
+        <v>16566.294300000001</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="2">
-        <v>16202.930700000001</v>
+      <c r="A144">
+        <v>16650.424200000001</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="2">
-        <v>16208.682199999999</v>
+      <c r="A145">
+        <v>16670.036800000002</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="2">
-        <v>16212.1746</v>
+      <c r="A146">
+        <v>16727.8488</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2">
-        <v>16230.056500000001</v>
+      <c r="A147">
+        <v>16730.0121</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="2">
-        <v>16236.088299999999</v>
+      <c r="A148">
+        <v>16757.646700000001</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="2">
-        <v>16240.4048</v>
+      <c r="A149">
+        <v>16804.2402</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="2">
-        <v>16250.900900000001</v>
+      <c r="A150">
+        <v>16974.548200000001</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="2">
-        <v>16285.2233</v>
+      <c r="A151">
+        <v>17015.747599999999</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="2">
-        <v>16289.221</v>
+      <c r="A152">
+        <v>17042.446899999999</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="2">
-        <v>16297.299199999999</v>
+      <c r="A153">
+        <v>17165.7965</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="2">
-        <v>16320.782999999999</v>
+      <c r="A154">
+        <v>17209.0026</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="2">
-        <v>16323.1594</v>
+      <c r="A155">
+        <v>17307.044600000001</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="2">
-        <v>16335.9908</v>
+      <c r="A156">
+        <v>17315.582600000002</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="2">
-        <v>16388.6201</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="2">
-        <v>16398.8704</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="2">
-        <v>16409.082399999999</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="2">
-        <v>16441.1165</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="2">
-        <v>16444.893599999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="2">
-        <v>16449.311000000002</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="2">
-        <v>16478.585599999999</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="2">
-        <v>16491.1731</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2">
-        <v>16521.740699999998</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="2">
-        <v>16543.713800000001</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="2">
-        <v>16556.518899999999</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="2">
-        <v>16566.294300000001</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="2">
-        <v>16650.424200000001</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="2">
-        <v>16670.036800000002</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="2">
-        <v>16727.8488</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="2">
-        <v>16729.264800000001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="2">
-        <v>16730.0121</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="2">
-        <v>16757.646700000001</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="2">
-        <v>16804.2402</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="2">
-        <v>16878.728200000001</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="2">
-        <v>16889.432700000001</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="2">
-        <v>16974.548200000001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="2">
-        <v>17010.094799999999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="2">
-        <v>17015.747599999999</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="2">
-        <v>17042.446899999999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="2">
-        <v>17137.616900000001</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="2">
-        <v>17165.7965</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="2">
-        <v>17170.886900000001</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="2">
-        <v>17209.0026</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="2">
-        <v>17307.044600000001</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="2">
-        <v>17315.582600000002</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="2">
+      <c r="A157">
         <v>17688.739699999998</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="2">
-        <v>17775.979599999999</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="2">
-        <v>20722.609799999998</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="2">
-        <v>21254.757600000001</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="2">
-        <v>21741.408599999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>